<commit_message>
Jævlig mange endringer som har blitt gjort for å kunne få time_window til å fungere
</commit_message>
<xml_diff>
--- a/Load_Profile/ramp/core/Appliances_and_users.xlsx
+++ b/Load_Profile/ramp/core/Appliances_and_users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsh\PycharmProjects\SizingOffGridMicrogrids\Load_Profile\ramp\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsh\PycharmProjects\SizingOffGridMicrogrids\Load_Profile\ramp\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA149CC5-C47E-488E-ADF9-8258AEED4957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B71640D-4BAE-4FDC-AADC-1167C1E8DBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DD404E9A-0D1E-45D4-8190-461235976194}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{DD404E9A-0D1E-45D4-8190-461235976194}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>A</t>
   </si>
@@ -117,533 +117,26 @@
     <t>PC</t>
   </si>
   <si>
-    <t>Fan</t>
-  </si>
-  <si>
     <t>visitor_hut_1,visitor_hut_2</t>
   </si>
   <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>1439</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFAA4926"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">r_w </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>0.35</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>23</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>59</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFAA4926"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">r_w </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>0.35</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>21</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>23</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>59</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>0.35</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6897BB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
-    <t>U</t>
+    <t>time_window</t>
+  </si>
+  <si>
+    <t>420,1439,r_w = 0.35</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFA9B7C6"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
     </font>
     <font>
       <b/>
@@ -661,19 +154,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF6897BB"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC7832"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFAA4926"/>
+      <color theme="1"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -715,16 +196,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1107,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A03B1C-7874-4F43-9A9A-C3425B424BF6}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:U3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1199,7 +680,7 @@
         <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -1216,7 +697,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1">
         <v>6</v>
@@ -1277,38 +758,12 @@
         <v>5</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>50</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
-        <f>4*60</f>
-        <v>240</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="K4" s="1">
-        <v>5</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="E4" s="5"/>
+      <c r="U4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>